<commit_message>
乌格拉利亚(Upgraliam) ALPHA 1.0.2 playtest 5支持
这个改版稳定性不好 不推荐大家去玩
</commit_message>
<xml_diff>
--- a/内部编号列表/[hack]R版.xlsx
+++ b/内部编号列表/[hack]R版.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7860"/>
+    <workbookView windowWidth="23040" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="1.4.6" sheetId="1" r:id="rId1"/>
@@ -5489,24 +5489,24 @@
   <sheetPr/>
   <dimension ref="A1:S98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="22.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.8796296296296" style="1" customWidth="1"/>
     <col min="4" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="20.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6296296296296" style="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="1"/>
-    <col min="9" max="9" width="23.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1296296296296" style="1" customWidth="1"/>
     <col min="10" max="12" width="9" style="1"/>
-    <col min="13" max="13" width="21.125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1296296296296" style="1" customWidth="1"/>
     <col min="14" max="15" width="9" style="1"/>
-    <col min="16" max="16" width="22.875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="22.8796296296296" style="1" customWidth="1"/>
     <col min="17" max="18" width="9" style="1"/>
-    <col min="19" max="19" width="18.125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="18.8888888888889" style="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>

</xml_diff>